<commit_message>
Adding star generation for T5 companions
</commit_message>
<xml_diff>
--- a/Traveller/class_diagram.xlsx
+++ b/Traveller/class_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\source\repos\Experiments\Traveller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2A32C5-FB6D-48D2-B2C3-DF4E99EDAAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BFB937-6D62-4D0B-B71D-D7C595DC6304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{E7D498D8-5C69-4151-B6A9-E1735E7CDADF}"/>
   </bookViews>
@@ -924,14 +924,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>farOrbits()</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-          </a:endParaRPr>
+            <a:t>createCompanionsFor()</a:t>
+          </a:r>
         </a:p>
         <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -961,7 +955,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>generateGasGiantCountFor()</a:t>
+            <a:t>farOrbits()</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:solidFill>
@@ -998,7 +992,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>availableOrbitsFor()</a:t>
+            <a:t>generateGasGiantCountFor()</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:solidFill>
@@ -1035,7 +1029,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>pruneInnerZoneFor()</a:t>
+            <a:t>availableOrbitsFor()</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:solidFill>
@@ -1072,48 +1066,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>keepOnlyInnerZoneFor()</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>generatePlanetoidBeltCountFor()</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>capturedPlanetsArePresentFor()</a:t>
+            <a:t>pruneInnerZoneFor()</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:solidFill>
@@ -1150,8 +1103,55 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>capturedPlanetQuantity()</a:t>
-          </a:r>
+            <a:t>keepOnlyInnerZoneFor()</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>generatePlanetoidBeltCountFor()</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>capturedPlanetsArePresentFor()</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -1181,7 +1181,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>placeGasGiantsFor()</a:t>
+            <a:t>capturedPlanetQuantity()</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1212,6 +1212,37 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
+            <a:t>placeGasGiantsFor()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>----------------</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
@@ -1220,17 +1251,6 @@
             </a:solidFill>
             <a:effectLst/>
           </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>createCompanionsFor()</a:t>
-          </a:r>
         </a:p>
         <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -3689,13 +3709,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>365124</xdr:colOff>
       <xdr:row>117</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>122</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3710,8 +3730,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="974724" y="21336000"/>
-          <a:ext cx="2441576" cy="806450"/>
+          <a:off x="974724" y="21332825"/>
+          <a:ext cx="2444751" cy="2108200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3787,18 +3807,148 @@
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
+            </a:rPr>
+            <a:t>new</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Primary()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
               <a:effectLst/>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>farOrbits()</a:t>
+            <a:t>----------------</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>createCompanionsFor()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>----------------</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
             <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -4267,7 +4417,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="H100" sqref="H100"/>
+      <selection activeCell="H88" sqref="H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>